<commit_message>
attempt to utilize flow limits
</commit_message>
<xml_diff>
--- a/offline/3_Bus.xlsx
+++ b/offline/3_Bus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\pyComms\offline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6535CB-56F1-42FD-A583-C59F981B13CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D885780D-1F12-4F81-9392-45D91FF502F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2A87A084-8292-0E46-981C-9D04D52D9924}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2A87A084-8292-0E46-981C-9D04D52D9924}"/>
   </bookViews>
   <sheets>
     <sheet name="Load Information" sheetId="1" r:id="rId1"/>
@@ -483,154 +483,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56AD0AC-1A9F-D540-B715-91722E643937}">
-  <dimension ref="C1:H33"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7">
-      <c r="C1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="3:7">
-      <c r="C2" s="1">
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="B2">
         <v>0</v>
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="3:7">
-      <c r="C3" s="1">
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="3:7">
-      <c r="C4" s="1">
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="B4">
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="3:7">
-      <c r="C5" s="1"/>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="3:7">
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="3:7">
-      <c r="C7" s="1"/>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="3:7">
-      <c r="C8" s="1"/>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="3:7">
-      <c r="C9" s="1"/>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="3:7">
-      <c r="C10" s="1"/>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="3:7">
-      <c r="C11" s="1"/>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="3:7">
-      <c r="C12" s="1"/>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="3:7">
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="3:7">
-      <c r="C14" s="1"/>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="3:7">
-      <c r="C15" s="1"/>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="3:7">
-      <c r="C16" s="1"/>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="3:8">
-      <c r="C17" s="1"/>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="3:8">
-      <c r="C18" s="1"/>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="3:8">
-      <c r="C19" s="1"/>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="3:8">
-      <c r="C20" s="1"/>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="3:8">
-      <c r="C21" s="1"/>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="3:8">
-      <c r="C22" s="1"/>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="3:8">
-      <c r="C23" s="1"/>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="3:8">
-      <c r="C24" s="1"/>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="3:8">
-      <c r="C25" s="1"/>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="3:8">
+    <row r="26" spans="1:8">
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="3:8">
+    <row r="27" spans="1:8">
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="3:8">
+    <row r="28" spans="1:8">
       <c r="F28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="3:8">
+    <row r="29" spans="1:8">
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="3:8">
+    <row r="30" spans="1:8">
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="3:8">
+    <row r="31" spans="1:8">
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="3:8">
+    <row r="32" spans="1:8">
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="8:8">
@@ -645,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E3B780-F058-194E-8684-15B5F1EF8C2B}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1417,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF22A77E-7842-8940-8B9A-F1FACC1ECEB2}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1465,11 +1465,11 @@
         <v>-57.1</v>
       </c>
       <c r="E2">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F39" si="0">E2+5</f>
-        <v>180</v>
+        <f t="shared" ref="F2:F4" si="0">E2+5</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1486,11 +1486,11 @@
         <v>-66.37</v>
       </c>
       <c r="E3">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1507,11 +1507,11 @@
         <v>-49.5</v>
       </c>
       <c r="E4">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6">

</xml_diff>